<commit_message>
Equivalent dividend, bond data
</commit_message>
<xml_diff>
--- a/data/sp-500-eps-est.xlsx
+++ b/data/sp-500-eps-est.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="1780" windowWidth="19340" windowHeight="13500" activeTab="2"/>
+    <workbookView xWindow="20620" yWindow="520" windowWidth="24880" windowHeight="15380"/>
   </bookViews>
   <sheets>
     <sheet name="ESTIMATES&amp;PEs" sheetId="1" r:id="rId1"/>
@@ -3767,7 +3767,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="13">
+  <numFmts count="14">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
@@ -3781,8 +3781,9 @@
     <numFmt numFmtId="174" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="175" formatCode="0.0%"/>
     <numFmt numFmtId="176" formatCode="[$-409]mmmm\-yy;@"/>
+    <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="71" x14ac:knownFonts="1">
+  <fonts count="72" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4255,6 +4256,12 @@
       <sz val="8.5"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="55">
@@ -4771,7 +4778,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="424">
+  <cellStyleXfs count="428">
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="171" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="171" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5205,8 +5212,12 @@
     <xf numFmtId="174" fontId="1" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="174" fontId="1" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="174" fontId="1" fillId="53" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="71" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="71" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="71" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="71" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="249">
+  <cellXfs count="250">
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -5766,8 +5777,11 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="424">
+  <cellStyles count="428">
     <cellStyle name="_x000a_bidires=100_x000d_" xfId="1"/>
     <cellStyle name="_x000a_bidires=100_x000d_ 2" xfId="103"/>
     <cellStyle name="_x000a_bidires=100_x000d_ 2 2" xfId="157"/>
@@ -6057,6 +6071,10 @@
     <cellStyle name="Explanatory Text 2 3" xfId="199"/>
     <cellStyle name="Explanatory Text 3" xfId="276"/>
     <cellStyle name="Explanatory Text 4" xfId="128"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="427" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="33" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Good 2" xfId="52"/>
     <cellStyle name="Good 2 2" xfId="298"/>
@@ -6497,8 +6515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y268"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A174" sqref="A174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -11869,7 +11887,7 @@
       <c r="K170" s="69"/>
     </row>
     <row r="171" spans="1:16">
-      <c r="A171" s="14">
+      <c r="A171" s="249">
         <v>38352</v>
       </c>
       <c r="B171" s="11">
@@ -11991,7 +12009,7 @@
       <c r="K174" s="69"/>
     </row>
     <row r="175" spans="1:16">
-      <c r="A175" s="14">
+      <c r="A175" s="249">
         <v>37986</v>
       </c>
       <c r="B175" s="11">
@@ -32999,9 +33017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>